<commit_message>
Updated units for Platelets and WBC after PhysioNet forum posting. Improve analysis.
</commit_message>
<xml_diff>
--- a/030-Descriptive-Stats/Laboratory-Values.xlsx
+++ b/030-Descriptive-Stats/Laboratory-Values.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Quantity</t>
   </si>
@@ -130,12 +130,6 @@
     <t>seconds</t>
   </si>
   <si>
-    <t>count/L</t>
-  </si>
-  <si>
-    <t>count/mL</t>
-  </si>
-  <si>
     <t>Measure of excess bicarbonate</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
     <t>Lactic acid</t>
   </si>
   <si>
-    <t>Total bilirubin</t>
-  </si>
-  <si>
     <t>Troponinl</t>
   </si>
   <si>
@@ -187,10 +178,34 @@
     <t>Leukocyte count</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Measure of acidity or basicity</t>
+  </si>
+  <si>
+    <t>count*10^3/µL</t>
+  </si>
+  <si>
+    <t>MaxPlotValue</t>
+  </si>
+  <si>
+    <t>MinPlotValue</t>
+  </si>
+  <si>
+    <t>RangeMin</t>
+  </si>
+  <si>
+    <t>RangeMax</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>http://idgateway.wustl.edu/Normal%20lab%20values.pdf</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Fraction_of_inspired_oxygen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total bilirubin </t>
   </si>
 </sst>
 </file>
@@ -542,21 +557,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N29" sqref="N29"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,8 +586,23 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -575,10 +610,16 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>-12</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -586,10 +627,25 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -597,21 +653,49 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>7.38</v>
+      </c>
+      <c r="E5">
+        <v>7.44</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>7.7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -619,10 +703,25 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>75</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -630,10 +729,25 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -641,10 +755,16 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -652,10 +772,25 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -663,10 +798,25 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>92</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>300</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -676,8 +826,14 @@
       <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -687,8 +843,14 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>85</v>
+      </c>
+      <c r="G12">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -698,8 +860,14 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -707,10 +875,16 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -718,10 +892,16 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -729,10 +909,16 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -742,8 +928,14 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -753,8 +945,14 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -764,8 +962,14 @@
       <c r="C19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -773,10 +977,16 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -784,10 +994,16 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -795,10 +1011,16 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="F22">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -806,10 +1028,16 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -817,21 +1045,33 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -841,16 +1081,28 @@
       <c r="C26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>